<commit_message>
modified:   .gitignore 	new file:   data/pics/pics.rar 	modified:   src/AC_Data.json 	modified:   src/greedy_Q.py 	modified:   src/test.xlsx
</commit_message>
<xml_diff>
--- a/src/test.xlsx
+++ b/src/test.xlsx
@@ -517,10 +517,10 @@
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="n">
-        <v>1352</v>
+        <v>1358</v>
       </c>
       <c r="K2" t="n">
-        <v>732</v>
+        <v>737</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
@@ -559,7 +559,7 @@
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="n">
-        <v>1629</v>
+        <v>1637</v>
       </c>
       <c r="K3" t="n">
         <v>255</v>
@@ -601,10 +601,10 @@
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="n">
-        <v>600</v>
+        <v>605</v>
       </c>
       <c r="K4" t="n">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
@@ -643,10 +643,10 @@
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="n">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="K5" t="n">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
@@ -811,7 +811,7 @@
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="n">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="K9" t="n">
         <v>0</v>
@@ -887,10 +887,10 @@
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="n">
-        <v>393</v>
+        <v>401</v>
       </c>
       <c r="K11" t="n">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="L11" t="inlineStr">
         <is>
@@ -963,10 +963,10 @@
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="n">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="K13" t="n">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="L13" t="inlineStr">
         <is>
@@ -1001,7 +1001,7 @@
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="n">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="K14" t="n">
         <v>119</v>
@@ -1191,10 +1191,10 @@
       <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="n">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="K19" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L19" t="inlineStr">
         <is>
@@ -1267,10 +1267,10 @@
       <c r="H21" t="inlineStr"/>
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="n">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="K21" t="n">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L21" t="inlineStr">
         <is>
@@ -1381,7 +1381,7 @@
       <c r="H24" t="inlineStr"/>
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="K24" t="n">
         <v>49</v>
@@ -2457,10 +2457,10 @@
       <c r="H50" t="inlineStr"/>
       <c r="I50" t="inlineStr"/>
       <c r="J50" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="K50" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L50" t="inlineStr">
         <is>
@@ -2877,10 +2877,10 @@
       <c r="H60" t="inlineStr"/>
       <c r="I60" t="inlineStr"/>
       <c r="J60" t="n">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="K60" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="L60" t="inlineStr">
         <is>

</xml_diff>